<commit_message>
Updated test data for invalid state sceanrio
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/BEFTA_Master_Definition_Invalid_Post_State.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/BEFTA_Master_Definition_Invalid_Post_State.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Desktop/RDM-9555/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C9018C-D9F3-744E-91DC-844F761A92C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8609B69D-E96D-1745-809D-A7C05BD57B0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -3076,7 +3076,7 @@
     <t>NoCActionInterpretationRequired</t>
   </si>
   <si>
-    <t>CaseApproved(TextField="showmethemoney" AND TextField3="showpage5"):1;CaseCreated(TextField="showmethemoney" AND TextField3="showpage5"):2;CaseModified</t>
+    <t>CaseApproved(TextField="showmethemoney" AND TextField3="showpage5"):1;CaseCreatedInvalid(TextField="showmethemoney" AND TextField3="showpage5"):2;CaseModified</t>
   </si>
 </sst>
 </file>
@@ -17777,7 +17777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C11" zoomScale="109" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C6" zoomScale="109" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>

</xml_diff>